<commit_message>
refined the time schedule
</commit_message>
<xml_diff>
--- a/Data/Schedule.xlsx
+++ b/Data/Schedule.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E45C1DAC-7B4D-4A10-A7DC-853F74B48C09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6924CAC9-306C-4FA1-B637-7EDD8B37DAA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -609,6 +609,33 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9">
       <alignment vertical="center"/>
     </xf>
@@ -617,33 +644,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1057,7 +1057,7 @@
   <dimension ref="B1:BO33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.25" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1095,66 +1095,66 @@
         <v>1</v>
       </c>
       <c r="J2" s="16"/>
-      <c r="K2" s="32" t="s">
+      <c r="K2" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="34"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="31"/>
       <c r="P2" s="17"/>
-      <c r="Q2" s="32" t="s">
+      <c r="Q2" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="R2" s="35"/>
-      <c r="S2" s="35"/>
-      <c r="T2" s="35"/>
-      <c r="U2" s="34"/>
+      <c r="R2" s="32"/>
+      <c r="S2" s="32"/>
+      <c r="T2" s="32"/>
+      <c r="U2" s="31"/>
       <c r="V2" s="18"/>
-      <c r="W2" s="29" t="s">
+      <c r="W2" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="X2" s="30"/>
-      <c r="Y2" s="36"/>
+      <c r="X2" s="26"/>
+      <c r="Y2" s="33"/>
       <c r="Z2" s="19"/>
-      <c r="AA2" s="29" t="s">
+      <c r="AA2" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="AB2" s="30"/>
-      <c r="AC2" s="30"/>
-      <c r="AD2" s="30"/>
-      <c r="AE2" s="30"/>
-      <c r="AF2" s="30"/>
+      <c r="AB2" s="26"/>
+      <c r="AC2" s="26"/>
+      <c r="AD2" s="26"/>
+      <c r="AE2" s="26"/>
+      <c r="AF2" s="26"/>
       <c r="AG2" s="20"/>
-      <c r="AH2" s="29" t="s">
+      <c r="AH2" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="AI2" s="30"/>
-      <c r="AJ2" s="30"/>
-      <c r="AK2" s="30"/>
-      <c r="AL2" s="30"/>
-      <c r="AM2" s="30"/>
-      <c r="AN2" s="30"/>
+      <c r="AI2" s="26"/>
+      <c r="AJ2" s="26"/>
+      <c r="AK2" s="26"/>
+      <c r="AL2" s="26"/>
+      <c r="AM2" s="26"/>
+      <c r="AN2" s="26"/>
       <c r="AO2" s="23"/>
       <c r="AP2" s="23"/>
     </row>
     <row r="3" spans="2:67" s="12" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="F3" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="31" t="s">
+      <c r="G3" s="27" t="s">
         <v>13</v>
       </c>
       <c r="H3" s="21" t="s">
@@ -1181,7 +1181,7 @@
       <c r="AA3" s="11"/>
     </row>
     <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="26"/>
+      <c r="B4" s="35"/>
       <c r="C4" s="28"/>
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
@@ -1482,7 +1482,7 @@
         <v>2</v>
       </c>
       <c r="D11" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
@@ -1531,10 +1531,10 @@
         <v>28</v>
       </c>
       <c r="C14" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D14" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E14" s="7">
         <v>1</v>
@@ -1619,10 +1619,10 @@
         <v>41</v>
       </c>
       <c r="C19" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D19" s="7">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
@@ -1683,7 +1683,7 @@
         <v>38</v>
       </c>
       <c r="C23" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D23" s="7">
         <v>5</v>
@@ -1699,7 +1699,7 @@
         <v>37</v>
       </c>
       <c r="C24" s="7">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D24" s="7">
         <v>8</v>
@@ -1715,7 +1715,7 @@
         <v>36</v>
       </c>
       <c r="C25" s="7">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D25" s="7">
         <v>2</v>
@@ -1811,24 +1811,24 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="2:2" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:2" ht="64.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="2" t="s">
         <v>42</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
     <mergeCell ref="AH2:AN2"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="K2:O2"/>
     <mergeCell ref="Q2:U2"/>
     <mergeCell ref="W2:Y2"/>
     <mergeCell ref="AA2:AF2"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
   </mergeCells>
   <conditionalFormatting sqref="B31:BO31">
     <cfRule type="expression" dxfId="9" priority="2">

</xml_diff>

<commit_message>
implemented basic log, working on catering-processing
</commit_message>
<xml_diff>
--- a/Data/Schedule.xlsx
+++ b/Data/Schedule.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F195A637-C6F8-4EA7-A68B-BF34A6A6937D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B4C3B71-78E7-4506-8A8E-9BB691E45191}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3855" yWindow="3855" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6090" yWindow="3390" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projektplanlægger" sheetId="1" r:id="rId1"/>
@@ -223,9 +223,6 @@
     <t>User API projekt</t>
   </si>
   <si>
-    <t>Catering API projekt</t>
-  </si>
-  <si>
     <t>got 19 days in total</t>
   </si>
   <si>
@@ -233,6 +230,9 @@
   </si>
   <si>
     <t>aiming for 18 days total used to have some breathingroom</t>
+  </si>
+  <si>
+    <t>Catering Dataproces projekt</t>
   </si>
 </sst>
 </file>
@@ -609,6 +609,33 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9">
       <alignment vertical="center"/>
     </xf>
@@ -617,33 +644,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1056,8 +1056,8 @@
   </sheetPr>
   <dimension ref="B1:BO33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="W20" sqref="W20"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.25" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1092,69 +1092,69 @@
         <v>12</v>
       </c>
       <c r="H2" s="15">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J2" s="16"/>
-      <c r="K2" s="32" t="s">
+      <c r="K2" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="34"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="31"/>
       <c r="P2" s="17"/>
-      <c r="Q2" s="32" t="s">
+      <c r="Q2" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="R2" s="35"/>
-      <c r="S2" s="35"/>
-      <c r="T2" s="35"/>
-      <c r="U2" s="34"/>
+      <c r="R2" s="32"/>
+      <c r="S2" s="32"/>
+      <c r="T2" s="32"/>
+      <c r="U2" s="31"/>
       <c r="V2" s="18"/>
-      <c r="W2" s="29" t="s">
+      <c r="W2" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="X2" s="30"/>
-      <c r="Y2" s="36"/>
+      <c r="X2" s="26"/>
+      <c r="Y2" s="33"/>
       <c r="Z2" s="19"/>
-      <c r="AA2" s="29" t="s">
+      <c r="AA2" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="AB2" s="30"/>
-      <c r="AC2" s="30"/>
-      <c r="AD2" s="30"/>
-      <c r="AE2" s="30"/>
-      <c r="AF2" s="30"/>
+      <c r="AB2" s="26"/>
+      <c r="AC2" s="26"/>
+      <c r="AD2" s="26"/>
+      <c r="AE2" s="26"/>
+      <c r="AF2" s="26"/>
       <c r="AG2" s="20"/>
-      <c r="AH2" s="29" t="s">
+      <c r="AH2" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="AI2" s="30"/>
-      <c r="AJ2" s="30"/>
-      <c r="AK2" s="30"/>
-      <c r="AL2" s="30"/>
-      <c r="AM2" s="30"/>
-      <c r="AN2" s="30"/>
+      <c r="AI2" s="26"/>
+      <c r="AJ2" s="26"/>
+      <c r="AK2" s="26"/>
+      <c r="AL2" s="26"/>
+      <c r="AM2" s="26"/>
+      <c r="AN2" s="26"/>
       <c r="AO2" s="23"/>
       <c r="AP2" s="23"/>
     </row>
     <row r="3" spans="2:67" s="12" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="25" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="27" t="s">
+      <c r="B3" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="F3" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="31" t="s">
+      <c r="G3" s="27" t="s">
         <v>13</v>
       </c>
       <c r="H3" s="21" t="s">
@@ -1181,7 +1181,7 @@
       <c r="AA3" s="11"/>
     </row>
     <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="26"/>
+      <c r="B4" s="35"/>
       <c r="C4" s="28"/>
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
@@ -1423,7 +1423,7 @@
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="8">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="8" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -1441,7 +1441,7 @@
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="8">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="9" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -1628,7 +1628,7 @@
     </row>
     <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C19" s="7">
         <v>3</v>
@@ -1680,10 +1680,10 @@
     </row>
     <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="6" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C22" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D22" s="7">
         <v>6</v>
@@ -1824,27 +1824,27 @@
     </row>
     <row r="32" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="33" spans="2:2" ht="64.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
     <mergeCell ref="AH2:AN2"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="K2:O2"/>
     <mergeCell ref="Q2:U2"/>
     <mergeCell ref="W2:Y2"/>
     <mergeCell ref="AA2:AF2"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
   </mergeCells>
   <conditionalFormatting sqref="B31:BO31">
     <cfRule type="expression" dxfId="9" priority="2">

</xml_diff>

<commit_message>
renamed some files, cleaned up, handling unhandled exceptions and shutdown in console, some code updates
</commit_message>
<xml_diff>
--- a/Data/Schedule.xlsx
+++ b/Data/Schedule.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E80B9D2-A840-44F3-81F5-03C9CDA0C746}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D3E6176-9F8C-458A-8B51-D39D68E03C39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -232,7 +232,7 @@
     <t>Kravspecifikationer update</t>
   </si>
   <si>
-    <t>Testspecifikationer iåpdate</t>
+    <t>Testspecifikationer update</t>
   </si>
 </sst>
 </file>
@@ -631,6 +631,18 @@
     <xf numFmtId="9" fontId="15" fillId="8" borderId="0" xfId="19" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="9" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -640,9 +652,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="10" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -657,15 +666,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="9" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="20">
@@ -1079,8 +1079,8 @@
   </sheetPr>
   <dimension ref="B1:AP33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.25" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1118,66 +1118,66 @@
         <v>8</v>
       </c>
       <c r="J2" s="16"/>
-      <c r="K2" s="32" t="s">
+      <c r="K2" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="34"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="36"/>
+      <c r="O2" s="37"/>
       <c r="P2" s="17"/>
-      <c r="Q2" s="32" t="s">
+      <c r="Q2" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="R2" s="35"/>
-      <c r="S2" s="35"/>
-      <c r="T2" s="35"/>
-      <c r="U2" s="34"/>
+      <c r="R2" s="38"/>
+      <c r="S2" s="38"/>
+      <c r="T2" s="38"/>
+      <c r="U2" s="37"/>
       <c r="V2" s="18"/>
-      <c r="W2" s="28" t="s">
+      <c r="W2" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="X2" s="29"/>
-      <c r="Y2" s="36"/>
+      <c r="X2" s="33"/>
+      <c r="Y2" s="39"/>
       <c r="Z2" s="19"/>
-      <c r="AA2" s="28" t="s">
+      <c r="AA2" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="AB2" s="29"/>
-      <c r="AC2" s="29"/>
-      <c r="AD2" s="29"/>
-      <c r="AE2" s="29"/>
-      <c r="AF2" s="29"/>
+      <c r="AB2" s="33"/>
+      <c r="AC2" s="33"/>
+      <c r="AD2" s="33"/>
+      <c r="AE2" s="33"/>
+      <c r="AF2" s="33"/>
       <c r="AG2" s="20"/>
-      <c r="AH2" s="28" t="s">
+      <c r="AH2" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="AI2" s="29"/>
-      <c r="AJ2" s="29"/>
-      <c r="AK2" s="29"/>
-      <c r="AL2" s="29"/>
-      <c r="AM2" s="29"/>
-      <c r="AN2" s="29"/>
+      <c r="AI2" s="33"/>
+      <c r="AJ2" s="33"/>
+      <c r="AK2" s="33"/>
+      <c r="AL2" s="33"/>
+      <c r="AM2" s="33"/>
+      <c r="AN2" s="33"/>
       <c r="AO2" s="23"/>
       <c r="AP2" s="23"/>
     </row>
     <row r="3" spans="2:42" s="12" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="37" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="39" t="s">
+      <c r="B3" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="39" t="s">
+      <c r="D3" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="39" t="s">
+      <c r="E3" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="39" t="s">
+      <c r="F3" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="30" t="s">
+      <c r="G3" s="34" t="s">
         <v>9</v>
       </c>
       <c r="H3" s="21" t="s">
@@ -1204,7 +1204,7 @@
       <c r="AA3" s="11"/>
     </row>
     <row r="4" spans="2:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="38"/>
+      <c r="B4" s="29"/>
       <c r="C4" s="31"/>
       <c r="D4" s="31"/>
       <c r="E4" s="31"/>
@@ -1799,17 +1799,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
     <mergeCell ref="AH2:AN2"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="K2:O2"/>
     <mergeCell ref="Q2:U2"/>
     <mergeCell ref="W2:Y2"/>
     <mergeCell ref="AA2:AF2"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
   </mergeCells>
   <conditionalFormatting sqref="B31:BO31">
     <cfRule type="expression" dxfId="9" priority="2">

</xml_diff>

<commit_message>
removed user orders and small changes
</commit_message>
<xml_diff>
--- a/Data/Schedule.xlsx
+++ b/Data/Schedule.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1611E0C2-0DCD-4962-9AAA-A52CA51C4FB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0531518-6DAF-4801-8080-FD77005CD4C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -631,6 +631,33 @@
     <xf numFmtId="9" fontId="15" fillId="8" borderId="0" xfId="19" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9">
       <alignment vertical="center"/>
     </xf>
@@ -639,33 +666,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="20">
@@ -1079,8 +1079,8 @@
   </sheetPr>
   <dimension ref="B1:AP33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="AR22" sqref="AR22"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.25" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1115,69 +1115,69 @@
         <v>8</v>
       </c>
       <c r="H2" s="15">
+        <v>12</v>
+      </c>
+      <c r="J2" s="16"/>
+      <c r="K2" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="16"/>
-      <c r="K2" s="35" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2" s="36"/>
-      <c r="M2" s="36"/>
-      <c r="N2" s="36"/>
-      <c r="O2" s="37"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="34"/>
       <c r="P2" s="17"/>
-      <c r="Q2" s="35" t="s">
+      <c r="Q2" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="R2" s="38"/>
-      <c r="S2" s="38"/>
-      <c r="T2" s="38"/>
-      <c r="U2" s="37"/>
+      <c r="R2" s="35"/>
+      <c r="S2" s="35"/>
+      <c r="T2" s="35"/>
+      <c r="U2" s="34"/>
       <c r="V2" s="18"/>
-      <c r="W2" s="32" t="s">
+      <c r="W2" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="X2" s="33"/>
-      <c r="Y2" s="39"/>
+      <c r="X2" s="29"/>
+      <c r="Y2" s="36"/>
       <c r="Z2" s="19"/>
-      <c r="AA2" s="32" t="s">
+      <c r="AA2" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="AB2" s="33"/>
-      <c r="AC2" s="33"/>
-      <c r="AD2" s="33"/>
-      <c r="AE2" s="33"/>
-      <c r="AF2" s="33"/>
+      <c r="AB2" s="29"/>
+      <c r="AC2" s="29"/>
+      <c r="AD2" s="29"/>
+      <c r="AE2" s="29"/>
+      <c r="AF2" s="29"/>
       <c r="AG2" s="20"/>
-      <c r="AH2" s="32" t="s">
+      <c r="AH2" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="AI2" s="33"/>
-      <c r="AJ2" s="33"/>
-      <c r="AK2" s="33"/>
-      <c r="AL2" s="33"/>
-      <c r="AM2" s="33"/>
-      <c r="AN2" s="33"/>
+      <c r="AI2" s="29"/>
+      <c r="AJ2" s="29"/>
+      <c r="AK2" s="29"/>
+      <c r="AL2" s="29"/>
+      <c r="AM2" s="29"/>
+      <c r="AN2" s="29"/>
       <c r="AO2" s="23"/>
       <c r="AP2" s="23"/>
     </row>
     <row r="3" spans="2:42" s="12" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="30" t="s">
+      <c r="B3" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="30" t="s">
+      <c r="D3" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="30" t="s">
+      <c r="E3" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="30" t="s">
+      <c r="F3" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="34" t="s">
+      <c r="G3" s="30" t="s">
         <v>9</v>
       </c>
       <c r="H3" s="21" t="s">
@@ -1204,7 +1204,7 @@
       <c r="AA3" s="11"/>
     </row>
     <row r="4" spans="2:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="29"/>
+      <c r="B4" s="38"/>
       <c r="C4" s="31"/>
       <c r="D4" s="31"/>
       <c r="E4" s="31"/>
@@ -1551,9 +1551,11 @@
       <c r="E18" s="7">
         <v>2</v>
       </c>
-      <c r="F18" s="7"/>
+      <c r="F18" s="7">
+        <v>11</v>
+      </c>
       <c r="G18" s="8">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="AA18"/>
     </row>
@@ -1811,17 +1813,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
     <mergeCell ref="AH2:AN2"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="K2:O2"/>
     <mergeCell ref="Q2:U2"/>
     <mergeCell ref="W2:Y2"/>
     <mergeCell ref="AA2:AF2"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
   </mergeCells>
   <conditionalFormatting sqref="B31:BO31">
     <cfRule type="expression" dxfId="9" priority="2">

</xml_diff>

<commit_message>
back-up of some data
</commit_message>
<xml_diff>
--- a/Data/Schedule.xlsx
+++ b/Data/Schedule.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0531518-6DAF-4801-8080-FD77005CD4C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDB79727-CA48-4B5E-9839-040C9977AE76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -631,6 +631,18 @@
     <xf numFmtId="9" fontId="15" fillId="8" borderId="0" xfId="19" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="9" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -640,9 +652,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="10" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -657,15 +666,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="9" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="20">
@@ -1080,7 +1080,7 @@
   <dimension ref="B1:AP33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.25" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1118,66 +1118,66 @@
         <v>12</v>
       </c>
       <c r="J2" s="16"/>
-      <c r="K2" s="32" t="s">
+      <c r="K2" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="34"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="36"/>
+      <c r="O2" s="37"/>
       <c r="P2" s="17"/>
-      <c r="Q2" s="32" t="s">
+      <c r="Q2" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="R2" s="35"/>
-      <c r="S2" s="35"/>
-      <c r="T2" s="35"/>
-      <c r="U2" s="34"/>
+      <c r="R2" s="38"/>
+      <c r="S2" s="38"/>
+      <c r="T2" s="38"/>
+      <c r="U2" s="37"/>
       <c r="V2" s="18"/>
-      <c r="W2" s="28" t="s">
+      <c r="W2" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="X2" s="29"/>
-      <c r="Y2" s="36"/>
+      <c r="X2" s="33"/>
+      <c r="Y2" s="39"/>
       <c r="Z2" s="19"/>
-      <c r="AA2" s="28" t="s">
+      <c r="AA2" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="AB2" s="29"/>
-      <c r="AC2" s="29"/>
-      <c r="AD2" s="29"/>
-      <c r="AE2" s="29"/>
-      <c r="AF2" s="29"/>
+      <c r="AB2" s="33"/>
+      <c r="AC2" s="33"/>
+      <c r="AD2" s="33"/>
+      <c r="AE2" s="33"/>
+      <c r="AF2" s="33"/>
       <c r="AG2" s="20"/>
-      <c r="AH2" s="28" t="s">
+      <c r="AH2" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="AI2" s="29"/>
-      <c r="AJ2" s="29"/>
-      <c r="AK2" s="29"/>
-      <c r="AL2" s="29"/>
-      <c r="AM2" s="29"/>
-      <c r="AN2" s="29"/>
+      <c r="AI2" s="33"/>
+      <c r="AJ2" s="33"/>
+      <c r="AK2" s="33"/>
+      <c r="AL2" s="33"/>
+      <c r="AM2" s="33"/>
+      <c r="AN2" s="33"/>
       <c r="AO2" s="23"/>
       <c r="AP2" s="23"/>
     </row>
     <row r="3" spans="2:42" s="12" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="37" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="39" t="s">
+      <c r="B3" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="39" t="s">
+      <c r="D3" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="39" t="s">
+      <c r="E3" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="39" t="s">
+      <c r="F3" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="30" t="s">
+      <c r="G3" s="34" t="s">
         <v>9</v>
       </c>
       <c r="H3" s="21" t="s">
@@ -1204,7 +1204,7 @@
       <c r="AA3" s="11"/>
     </row>
     <row r="4" spans="2:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="38"/>
+      <c r="B4" s="29"/>
       <c r="C4" s="31"/>
       <c r="D4" s="31"/>
       <c r="E4" s="31"/>
@@ -1326,7 +1326,7 @@
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="8">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="AA7"/>
     </row>
@@ -1345,7 +1345,7 @@
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="8">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="AA8"/>
     </row>
@@ -1572,9 +1572,11 @@
       <c r="E19" s="7">
         <v>2</v>
       </c>
-      <c r="F19" s="7"/>
+      <c r="F19" s="7">
+        <v>10</v>
+      </c>
       <c r="G19" s="8">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="AA19"/>
     </row>
@@ -1813,17 +1815,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
     <mergeCell ref="AH2:AN2"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="K2:O2"/>
     <mergeCell ref="Q2:U2"/>
     <mergeCell ref="W2:Y2"/>
     <mergeCell ref="AA2:AF2"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
   </mergeCells>
   <conditionalFormatting sqref="B31:BO31">
     <cfRule type="expression" dxfId="9" priority="2">

</xml_diff>

<commit_message>
schedule update and minor changes to usercontract
</commit_message>
<xml_diff>
--- a/Data/Schedule.xlsx
+++ b/Data/Schedule.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8066FBC-0176-4D77-B714-C22A51D5CE17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1D3A5AF-D394-4E16-AC0E-30EB88D60D1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -631,6 +631,18 @@
     <xf numFmtId="9" fontId="15" fillId="8" borderId="0" xfId="19" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="9" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -640,9 +652,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="10" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -657,15 +666,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="9" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="20">
@@ -1080,7 +1080,7 @@
   <dimension ref="B1:AP33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="AJ10" sqref="AJ10"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.25" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1118,66 +1118,66 @@
         <v>13</v>
       </c>
       <c r="J2" s="16"/>
-      <c r="K2" s="32" t="s">
+      <c r="K2" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="34"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="36"/>
+      <c r="O2" s="37"/>
       <c r="P2" s="17"/>
-      <c r="Q2" s="32" t="s">
+      <c r="Q2" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="R2" s="35"/>
-      <c r="S2" s="35"/>
-      <c r="T2" s="35"/>
-      <c r="U2" s="34"/>
+      <c r="R2" s="38"/>
+      <c r="S2" s="38"/>
+      <c r="T2" s="38"/>
+      <c r="U2" s="37"/>
       <c r="V2" s="18"/>
-      <c r="W2" s="28" t="s">
+      <c r="W2" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="X2" s="29"/>
-      <c r="Y2" s="36"/>
+      <c r="X2" s="33"/>
+      <c r="Y2" s="39"/>
       <c r="Z2" s="19"/>
-      <c r="AA2" s="28" t="s">
+      <c r="AA2" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="AB2" s="29"/>
-      <c r="AC2" s="29"/>
-      <c r="AD2" s="29"/>
-      <c r="AE2" s="29"/>
-      <c r="AF2" s="29"/>
+      <c r="AB2" s="33"/>
+      <c r="AC2" s="33"/>
+      <c r="AD2" s="33"/>
+      <c r="AE2" s="33"/>
+      <c r="AF2" s="33"/>
       <c r="AG2" s="20"/>
-      <c r="AH2" s="28" t="s">
+      <c r="AH2" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="AI2" s="29"/>
-      <c r="AJ2" s="29"/>
-      <c r="AK2" s="29"/>
-      <c r="AL2" s="29"/>
-      <c r="AM2" s="29"/>
-      <c r="AN2" s="29"/>
+      <c r="AI2" s="33"/>
+      <c r="AJ2" s="33"/>
+      <c r="AK2" s="33"/>
+      <c r="AL2" s="33"/>
+      <c r="AM2" s="33"/>
+      <c r="AN2" s="33"/>
       <c r="AO2" s="23"/>
       <c r="AP2" s="23"/>
     </row>
     <row r="3" spans="2:42" s="12" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="37" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="39" t="s">
+      <c r="B3" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="39" t="s">
+      <c r="D3" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="39" t="s">
+      <c r="E3" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="39" t="s">
+      <c r="F3" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="30" t="s">
+      <c r="G3" s="34" t="s">
         <v>9</v>
       </c>
       <c r="H3" s="21" t="s">
@@ -1204,7 +1204,7 @@
       <c r="AA3" s="11"/>
     </row>
     <row r="4" spans="2:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="38"/>
+      <c r="B4" s="29"/>
       <c r="C4" s="31"/>
       <c r="D4" s="31"/>
       <c r="E4" s="31"/>
@@ -1345,7 +1345,7 @@
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="8">
-        <v>0.7</v>
+        <v>0.95</v>
       </c>
       <c r="AA8"/>
     </row>
@@ -1815,17 +1815,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
     <mergeCell ref="AH2:AN2"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="K2:O2"/>
     <mergeCell ref="Q2:U2"/>
     <mergeCell ref="W2:Y2"/>
     <mergeCell ref="AA2:AF2"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
   </mergeCells>
   <conditionalFormatting sqref="B31:BO31">
     <cfRule type="expression" dxfId="9" priority="2">

</xml_diff>

<commit_message>
updated schedule and added reports for backup
</commit_message>
<xml_diff>
--- a/Data/Schedule.xlsx
+++ b/Data/Schedule.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A7043BD-98CB-4F7E-993E-730F4128DDA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16FC86EE-D2E6-447F-BEDE-E14AD03F1EFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -628,6 +628,33 @@
     <xf numFmtId="9" fontId="15" fillId="8" borderId="0" xfId="19" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9">
       <alignment vertical="center"/>
     </xf>
@@ -636,33 +663,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="20">
@@ -1077,7 +1077,7 @@
   <dimension ref="B1:AP32"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="AJ12" sqref="AJ12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.25" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1114,69 +1114,69 @@
         <v>7</v>
       </c>
       <c r="H2" s="15">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="J2" s="16"/>
-      <c r="K2" s="35" t="s">
+      <c r="K2" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="36"/>
-      <c r="M2" s="36"/>
-      <c r="N2" s="36"/>
-      <c r="O2" s="37"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="34"/>
       <c r="P2" s="17"/>
-      <c r="Q2" s="35" t="s">
+      <c r="Q2" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="R2" s="38"/>
-      <c r="S2" s="38"/>
-      <c r="T2" s="38"/>
-      <c r="U2" s="37"/>
+      <c r="R2" s="35"/>
+      <c r="S2" s="35"/>
+      <c r="T2" s="35"/>
+      <c r="U2" s="34"/>
       <c r="V2" s="18"/>
-      <c r="W2" s="32" t="s">
+      <c r="W2" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="X2" s="33"/>
-      <c r="Y2" s="39"/>
+      <c r="X2" s="29"/>
+      <c r="Y2" s="36"/>
       <c r="Z2" s="19"/>
-      <c r="AA2" s="32" t="s">
+      <c r="AA2" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="AB2" s="33"/>
-      <c r="AC2" s="33"/>
-      <c r="AD2" s="33"/>
-      <c r="AE2" s="33"/>
-      <c r="AF2" s="33"/>
+      <c r="AB2" s="29"/>
+      <c r="AC2" s="29"/>
+      <c r="AD2" s="29"/>
+      <c r="AE2" s="29"/>
+      <c r="AF2" s="29"/>
       <c r="AG2" s="20"/>
-      <c r="AH2" s="32" t="s">
+      <c r="AH2" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="AI2" s="33"/>
-      <c r="AJ2" s="33"/>
-      <c r="AK2" s="33"/>
-      <c r="AL2" s="33"/>
-      <c r="AM2" s="33"/>
-      <c r="AN2" s="33"/>
+      <c r="AI2" s="29"/>
+      <c r="AJ2" s="29"/>
+      <c r="AK2" s="29"/>
+      <c r="AL2" s="29"/>
+      <c r="AM2" s="29"/>
+      <c r="AN2" s="29"/>
       <c r="AO2" s="23"/>
       <c r="AP2" s="23"/>
     </row>
     <row r="3" spans="2:42" s="12" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="30" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="30" t="s">
+      <c r="B3" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="30" t="s">
+      <c r="E3" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="30" t="s">
+      <c r="F3" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="34" t="s">
+      <c r="G3" s="30" t="s">
         <v>8</v>
       </c>
       <c r="H3" s="21" t="s">
@@ -1203,7 +1203,7 @@
       <c r="AA3" s="11"/>
     </row>
     <row r="4" spans="2:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="29"/>
+      <c r="B4" s="38"/>
       <c r="C4" s="31"/>
       <c r="D4" s="31"/>
       <c r="E4" s="31"/>
@@ -1323,9 +1323,11 @@
       <c r="E7" s="7">
         <v>1</v>
       </c>
-      <c r="F7" s="7"/>
+      <c r="F7" s="7">
+        <v>18</v>
+      </c>
       <c r="G7" s="8">
-        <v>0.98</v>
+        <v>1</v>
       </c>
       <c r="AA7"/>
     </row>
@@ -1342,9 +1344,11 @@
       <c r="E8" s="7">
         <v>1</v>
       </c>
-      <c r="F8" s="7"/>
+      <c r="F8" s="7">
+        <v>18</v>
+      </c>
       <c r="G8" s="8">
-        <v>0.98</v>
+        <v>1</v>
       </c>
       <c r="AA8"/>
     </row>
@@ -1797,17 +1801,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
     <mergeCell ref="AH2:AN2"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="K2:O2"/>
     <mergeCell ref="Q2:U2"/>
     <mergeCell ref="W2:Y2"/>
     <mergeCell ref="AA2:AF2"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
   </mergeCells>
   <conditionalFormatting sqref="B30:BO30">
     <cfRule type="expression" dxfId="9" priority="2">

</xml_diff>